<commit_message>
added expiration in food data
</commit_message>
<xml_diff>
--- a/php/Data/FoodData.xlsx
+++ b/php/Data/FoodData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{2BBA6306-D104-40F9-AABA-27598544916B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E8AA4755-9880-4960-AC74-5DB43F55E22A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>Rice</t>
+  </si>
+  <si>
+    <t>Expiration </t>
   </si>
 </sst>
 </file>
@@ -389,18 +392,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="9.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -419,8 +424,11 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -439,8 +447,11 @@
       <c r="F2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -459,8 +470,11 @@
       <c r="F3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -479,8 +493,11 @@
       <c r="F4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -499,8 +516,11 @@
       <c r="F5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -519,8 +539,11 @@
       <c r="F6">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -539,8 +562,11 @@
       <c r="F7">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -559,8 +585,11 @@
       <c r="F8">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -579,8 +608,11 @@
       <c r="F9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -598,6 +630,9 @@
       </c>
       <c r="F10">
         <v>0</v>
+      </c>
+      <c r="G10">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>